<commit_message>
Format and Build Fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/jenkins-test-data.xlsx
+++ b/src/test/resources/jenkins-test-data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>test_service_provider</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Windows</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
   <si>
     <t>1920x1080</t>
@@ -104,7 +107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -115,17 +118,6 @@
       <name val="Arial"/>
     </font>
     <font/>
-    <font>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF999999"/>
-      <name val="Inherit"/>
-    </font>
-    <font>
-      <color rgb="FF708090"/>
-      <name val="Inherit"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,33 +133,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -384,15 +358,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="19.29"/>
-    <col customWidth="1" min="5" max="5" width="30.0"/>
-    <col customWidth="1" min="6" max="6" width="16.71"/>
-    <col customWidth="1" min="7" max="7" width="17.43"/>
-    <col customWidth="1" min="8" max="8" width="19.86"/>
-    <col customWidth="1" min="9" max="9" width="16.0"/>
-    <col customWidth="1" min="12" max="12" width="27.86"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -433,152 +398,118 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f>TEXT(10,0)</f>
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2">
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1">
         <v>30.0</v>
       </c>
-      <c r="J2" s="2" t="b">
+      <c r="J2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="J3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="2">
-        <v>30.0</v>
-      </c>
-      <c r="J3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="1">
+        <v>30.0</v>
+      </c>
+      <c r="J4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="5">
-        <v>30.0</v>
-      </c>
-      <c r="J4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="17">
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18">
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19">
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20">
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21">
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22">
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23">
-      <c r="D23" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>